<commit_message>
Generating a new excel sheet with the results of sent messages, whether it was sent or not.
</commit_message>
<xml_diff>
--- a/Planilha_TESTE.xlsx
+++ b/Planilha_TESTE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python Projects\Automatic WhatsApp - Copia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8B9FC6-DEB5-4215-8B3E-12A517C8AA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7635B67-DC81-4635-B933-8A1F56EC0BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11295" xr2:uid="{AD29BEF3-0AEA-4D89-85D9-C05B98C02434}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD29BEF3-0AEA-4D89-85D9-C05B98C02434}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Numero</t>
   </si>
@@ -45,25 +45,16 @@
     <t>Lucas LTDA</t>
   </si>
   <si>
-    <t>Jose EIRELI</t>
-  </si>
-  <si>
-    <t>Pedro LTDA</t>
-  </si>
-  <si>
-    <t>Matheus S.A</t>
-  </si>
-  <si>
-    <t>7993493-6581</t>
-  </si>
-  <si>
-    <t>2090047-0338</t>
-  </si>
-  <si>
-    <t>5397776-1174</t>
-  </si>
-  <si>
-    <t>2394029-1578</t>
+    <t>62992690601</t>
+  </si>
+  <si>
+    <t>Felipe Rocha</t>
+  </si>
+  <si>
+    <t>6233571219</t>
+  </si>
+  <si>
+    <t>Situação</t>
   </si>
 </sst>
 </file>
@@ -429,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531E7FEC-9B49-4A0D-8C50-0B5ECB52DD67}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -443,44 +434,31 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Except and Sheet
</commit_message>
<xml_diff>
--- a/Planilha_TESTE.xlsx
+++ b/Planilha_TESTE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python Projects\Automatic WhatsApp - Copia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DCB37A-139B-4DD9-B904-259BD918B566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9507D00-FD79-4632-A331-8ADD1386EF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD29BEF3-0AEA-4D89-85D9-C05B98C02434}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Numero</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>Lucas LTDA</t>
-  </si>
-  <si>
-    <t>62992690601</t>
-  </si>
-  <si>
-    <t>6233571219</t>
   </si>
   <si>
     <t>Situação</t>
@@ -61,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +64,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -97,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -105,6 +107,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,7 +428,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -442,24 +447,20 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>